<commit_message>
Setup for US-NR1 test run
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\SCOPE\SCOPE_v1.72\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnorton/Models/SCOPE/SCOPE_v1.73/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD202D0-ED6A-354F-AC88-C73D6B8EE836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8892" windowHeight="5196" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21160" windowHeight="15240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -17,12 +18,20 @@
     <sheet name="filenames" sheetId="3" r:id="rId3"/>
     <sheet name="inputdata" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="347">
   <si>
     <t>Cab</t>
   </si>
@@ -195,9 +204,6 @@
     <t>The_following_are_only_for_the_time_series_option!</t>
   </si>
   <si>
-    <t>for_verification</t>
-  </si>
-  <si>
     <t>t_file</t>
   </si>
   <si>
@@ -303,22 +309,7 @@
     <t>FLEX-S3_std.atm</t>
   </si>
   <si>
-    <t>t_.dat</t>
-  </si>
-  <si>
     <t>year_.dat</t>
-  </si>
-  <si>
-    <t>Rin_.dat</t>
-  </si>
-  <si>
-    <t>Rli_.dat</t>
-  </si>
-  <si>
-    <t>p_.dat</t>
-  </si>
-  <si>
-    <t>Ta_.dat</t>
   </si>
   <si>
     <t>ea_.dat</t>
@@ -1259,9 +1250,6 @@
     <t>BSMBrightness</t>
   </si>
   <si>
-    <t>verification_run</t>
-  </si>
-  <si>
     <t>LIDF_file</t>
   </si>
   <si>
@@ -1269,12 +1257,33 @@
   </si>
   <si>
     <t>optional_(leave_empty_for_calculations_based_on_t_file_year_timezn)</t>
+  </si>
+  <si>
+    <t>doy_.dat</t>
+  </si>
+  <si>
+    <t>sw_.dat</t>
+  </si>
+  <si>
+    <t>lw_.dat</t>
+  </si>
+  <si>
+    <t>ps_.dat</t>
+  </si>
+  <si>
+    <t>ta_.dat</t>
+  </si>
+  <si>
+    <t>lai_constant_.dat</t>
+  </si>
+  <si>
+    <t>US-NR1-2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1813,6 +1822,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1848,6 +1874,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2023,320 +2066,320 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J96"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0"/>
+    <sheetView topLeftCell="A54" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>82</v>
       </c>
-      <c r="C18" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C20" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>84</v>
-      </c>
       <c r="C21" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>54</v>
       </c>
       <c r="C24" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>59</v>
       </c>
-      <c r="C26" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C36" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="C39" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="37" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="37" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="36" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="52" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C56" s="52" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="53"/>
       <c r="B57" s="53"/>
       <c r="C57" s="53"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B58" s="11">
         <v>1</v>
@@ -2345,9 +2388,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B59" s="11">
         <v>-1</v>
@@ -2356,9 +2399,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B60" s="11">
         <v>0</v>
@@ -2367,9 +2410,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B61" s="11">
         <v>0</v>
@@ -2378,9 +2421,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B62" s="11">
         <v>-0.35</v>
@@ -2389,9 +2432,9 @@
         <v>-0.15</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B63" s="12">
         <v>0</v>
@@ -2400,16 +2443,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="36" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="15"/>
       <c r="B68" s="16"/>
       <c r="C68" s="54" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D68" s="55"/>
       <c r="E68" s="55"/>
@@ -2419,44 +2462,44 @@
       <c r="I68" s="17"/>
       <c r="J68" s="18"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B69" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C69" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="G69" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="H69" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="I69" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="D69" s="22" t="s">
+      <c r="J69" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="E69" s="22" t="s">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="F69" s="22" t="s">
+      <c r="B70" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="G69" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="H69" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="I69" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="J69" s="23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="C70" s="25">
         <v>0.2</v>
@@ -2483,12 +2526,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="24" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C71" s="25">
         <v>0.2</v>
@@ -2515,12 +2558,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C72" s="25">
         <v>0.2</v>
@@ -2547,12 +2590,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C73" s="25">
         <v>0.2</v>
@@ -2579,12 +2622,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="24" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C74" s="25">
         <v>0.2</v>
@@ -2611,12 +2654,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="24" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C75" s="25">
         <v>0.2</v>
@@ -2643,12 +2686,12 @@
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="24" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C76" s="25">
         <v>0.2</v>
@@ -2675,12 +2718,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="24" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C77" s="25">
         <v>0.2</v>
@@ -2707,12 +2750,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="24" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C78" s="25">
         <v>0.2</v>
@@ -2739,12 +2782,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="24" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C79" s="25">
         <v>0.2</v>
@@ -2771,12 +2814,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="24" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C80" s="25">
         <v>0.2</v>
@@ -2803,12 +2846,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="24" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="C81" s="25">
         <v>0.2</v>
@@ -2835,12 +2878,12 @@
         <v>360</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="31" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B82" s="32" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C82" s="33">
         <v>0.2</v>
@@ -2867,40 +2910,40 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="36" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B86" s="41" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C86" s="41" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D86" s="41" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E86" s="41" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="F86" s="41" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="39" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="B87" s="39" t="s">
         <v>11</v>
       </c>
       <c r="C87" s="39" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D87" s="42">
         <v>1000</v>
@@ -2913,15 +2956,15 @@
       </c>
       <c r="G87" s="43"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="39" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="B88" s="39" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="C88" s="39" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D88" s="42">
         <v>209</v>
@@ -2934,15 +2977,15 @@
       </c>
       <c r="G88" s="43"/>
     </row>
-    <row r="89" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A89" s="39" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B89" s="39" t="s">
         <v>21</v>
       </c>
       <c r="C89" s="39" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D89" s="43">
         <v>1.4999999999999999E-2</v>
@@ -2955,15 +2998,15 @@
       </c>
       <c r="G89" s="43"/>
     </row>
-    <row r="90" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A90" s="39" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="B90" s="39" t="s">
         <v>17</v>
       </c>
       <c r="C90" s="39" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D90" s="43">
         <v>7</v>
@@ -2976,36 +3019,36 @@
       </c>
       <c r="G90" s="43"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="39" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B91" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C91" s="39" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D91" s="42" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E91" s="42" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="F91" s="42" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="G91" s="42"/>
     </row>
-    <row r="92" spans="1:10" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" ht="19" x14ac:dyDescent="0.2">
       <c r="A92" s="39" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B92" s="39" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C92" s="39" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D92" s="42">
         <v>380</v>
@@ -3017,18 +3060,18 @@
         <v>500</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A93" s="39" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C93" s="39" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D93" s="42" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E93" s="42">
         <v>0</v>
@@ -3037,15 +3080,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A94" s="39" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B94" s="39" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C94" s="39" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D94" s="42">
         <v>1</v>
@@ -3057,15 +3100,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A95" s="44" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B95" s="44" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C95" s="44" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D95" s="45">
         <v>0</v>
@@ -3077,15 +3120,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="46" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B96" s="46" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C96" s="46" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D96" s="47">
         <v>1</v>
@@ -3111,211 +3154,211 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="1" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
         <v>88</v>
       </c>
-      <c r="E5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E10" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E11" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="E14" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
         <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
@@ -3324,7 +3367,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3332,18 +3375,18 @@
         <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="E23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3354,206 +3397,209 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>82</v>
       </c>
-      <c r="B4" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>83</v>
       </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>91</v>
       </c>
-      <c r="B6" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>58</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>59</v>
       </c>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="51" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="50" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="49"/>
     </row>
   </sheetData>
@@ -3564,91 +3610,91 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:DV89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="8" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="8" width="9.1640625" customWidth="1"/>
     <col min="9" max="9" width="40.33203125" customWidth="1"/>
-    <col min="10" max="26" width="9.109375" customWidth="1"/>
-    <col min="27" max="27" width="9.109375" style="4" customWidth="1"/>
-    <col min="28" max="28" width="24.5546875" customWidth="1"/>
+    <col min="10" max="26" width="9.1640625" customWidth="1"/>
+    <col min="27" max="27" width="9.1640625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="AA6" s="8"/>
       <c r="AB6" s="5"/>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AA9"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>6.25</v>
       </c>
       <c r="H10" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I10" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="AA10"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -3656,14 +3702,14 @@
         <v>1.2E-2</v>
       </c>
       <c r="H11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="I11" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="AA11"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3671,14 +3717,14 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="H12" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="I12" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="AA12"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -3686,29 +3732,29 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="I13" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AA13"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="I14" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="AA14"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -3716,14 +3762,14 @@
         <v>1.4</v>
       </c>
       <c r="H15" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="I15" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="AA15"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3732,11 +3778,11 @@
       </c>
       <c r="E16" s="13"/>
       <c r="I16" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AA16"/>
     </row>
-    <row r="17" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -3744,34 +3790,34 @@
         <v>0.01</v>
       </c>
       <c r="I17" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="AA17"/>
     </row>
-    <row r="18" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:103" x14ac:dyDescent="0.2">
       <c r="AA18"/>
     </row>
-    <row r="19" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:103" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="H20" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="I20" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="AA20"/>
     </row>
-    <row r="21" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -3779,7 +3825,7 @@
         <v>8</v>
       </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="AB21" s="9"/>
       <c r="AZ21" s="4"/>
@@ -3789,12 +3835,12 @@
       <c r="CX21" s="4"/>
       <c r="CY21" s="9"/>
     </row>
-    <row r="22" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B22">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="AB22" s="9"/>
       <c r="AZ22" s="4"/>
@@ -3804,7 +3850,7 @@
       <c r="CX22" s="4"/>
       <c r="CY22" s="9"/>
     </row>
-    <row r="23" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -3812,7 +3858,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="AB23" s="9"/>
       <c r="AZ23" s="4"/>
@@ -3822,7 +3868,7 @@
       <c r="CX23" s="4"/>
       <c r="CY23" s="9"/>
     </row>
-    <row r="24" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -3830,11 +3876,11 @@
         <v>0.63959999999999995</v>
       </c>
       <c r="I24" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="AA24"/>
     </row>
-    <row r="25" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -3842,7 +3888,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I25" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="AB25" s="9"/>
       <c r="AZ25" s="4"/>
@@ -3852,7 +3898,7 @@
       <c r="CX25" s="4"/>
       <c r="CY25" s="9"/>
     </row>
-    <row r="26" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -3872,105 +3918,105 @@
         <v>328</v>
       </c>
       <c r="I26" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="AZ26" s="4"/>
       <c r="BY26" s="4"/>
       <c r="CX26" s="4"/>
     </row>
-    <row r="27" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="28" spans="1:103" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B28">
         <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="I28" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="AZ28" s="4"/>
       <c r="BY28" s="4"/>
       <c r="CX28" s="4"/>
     </row>
-    <row r="29" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B29">
         <v>0.50700000000000001</v>
       </c>
       <c r="H29" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="I29" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="AZ29" s="4"/>
       <c r="BY29" s="4"/>
       <c r="CX29" s="4"/>
     </row>
-    <row r="30" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="I30" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="AZ30" s="4"/>
       <c r="BY30" s="4"/>
       <c r="CX30" s="4"/>
     </row>
-    <row r="31" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="I31" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="AZ31" s="4"/>
       <c r="BY31" s="4"/>
       <c r="CX31" s="4"/>
     </row>
-    <row r="32" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="AZ32" s="4"/>
       <c r="BY32" s="4"/>
       <c r="CX32" s="4"/>
     </row>
-    <row r="33" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:103" x14ac:dyDescent="0.2">
       <c r="AZ33" s="4"/>
       <c r="BY33" s="4"/>
       <c r="CX33" s="4"/>
     </row>
-    <row r="34" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
@@ -3979,7 +4025,7 @@
       <c r="BY34" s="7"/>
       <c r="CX34" s="7"/>
     </row>
-    <row r="35" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3988,7 +4034,7 @@
       </c>
       <c r="G35" s="13"/>
       <c r="I35" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="AB35" s="9"/>
       <c r="AZ35" s="4"/>
@@ -3998,12 +4044,12 @@
       <c r="CX35" s="4"/>
       <c r="CY35" s="9"/>
     </row>
-    <row r="36" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:103" x14ac:dyDescent="0.2">
       <c r="AZ36" s="4"/>
       <c r="BY36" s="4"/>
       <c r="CX36" s="4"/>
     </row>
-    <row r="37" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
@@ -4012,7 +4058,7 @@
       <c r="BY37" s="7"/>
       <c r="CX37" s="7"/>
     </row>
-    <row r="38" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>27</v>
       </c>
@@ -4020,13 +4066,13 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="AZ38" s="4"/>
       <c r="BY38" s="4"/>
       <c r="CX38" s="4"/>
     </row>
-    <row r="39" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>28</v>
       </c>
@@ -4034,16 +4080,16 @@
         <v>500</v>
       </c>
       <c r="H39" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I39" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="AZ39" s="4"/>
       <c r="BY39" s="4"/>
       <c r="CX39" s="4"/>
     </row>
-    <row r="40" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -4051,13 +4097,13 @@
         <v>0.06</v>
       </c>
       <c r="I40" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="AZ40" s="4"/>
       <c r="BY40" s="4"/>
       <c r="CX40" s="4"/>
     </row>
-    <row r="41" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -4065,16 +4111,16 @@
         <v>1180</v>
       </c>
       <c r="H41" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="I41" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="AZ41" s="4"/>
       <c r="BY41" s="4"/>
       <c r="CX41" s="4"/>
     </row>
-    <row r="42" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -4082,16 +4128,16 @@
         <v>1800</v>
       </c>
       <c r="H42" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I42" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="AZ42" s="4"/>
       <c r="BY42" s="4"/>
       <c r="CX42" s="4"/>
     </row>
-    <row r="43" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -4099,77 +4145,77 @@
         <v>1.55</v>
       </c>
       <c r="H43" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="I43" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="AZ43" s="4"/>
       <c r="BY43" s="4"/>
       <c r="CX43" s="4"/>
     </row>
-    <row r="44" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B44">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I44" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="AZ44" s="4"/>
       <c r="BY44" s="4"/>
       <c r="CX44" s="4"/>
     </row>
-    <row r="45" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B45">
         <v>0.5</v>
       </c>
       <c r="I45" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="AZ45" s="4"/>
       <c r="BY45" s="4"/>
       <c r="CX45" s="4"/>
     </row>
-    <row r="46" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B46">
         <v>25</v>
       </c>
       <c r="I46" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="AZ46" s="4"/>
       <c r="BY46" s="4"/>
       <c r="CX46" s="4"/>
     </row>
-    <row r="47" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B47">
         <v>45</v>
       </c>
       <c r="I47" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="AZ47" s="4"/>
       <c r="BY47" s="4"/>
       <c r="CX47" s="4"/>
     </row>
-    <row r="48" spans="1:103" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:103" x14ac:dyDescent="0.2">
       <c r="AZ48" s="4"/>
       <c r="BY48" s="4"/>
       <c r="CX48" s="4"/>
     </row>
-    <row r="49" spans="1:126" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:126" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>3</v>
       </c>
@@ -4178,18 +4224,18 @@
       <c r="BY49" s="7"/>
       <c r="CX49" s="7"/>
     </row>
-    <row r="50" spans="1:126" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I50" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="AB50" s="4"/>
       <c r="AC50" s="4"/>
@@ -4291,24 +4337,24 @@
       <c r="DU50" s="4"/>
       <c r="DV50" s="4"/>
     </row>
-    <row r="51" spans="1:126" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>24</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H51" t="s">
         <v>17</v>
       </c>
       <c r="I51" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AB51" s="9"/>
     </row>
-    <row r="52" spans="1:126" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B52">
         <v>-0.35</v>
@@ -4317,14 +4363,14 @@
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
       <c r="I52" s="11" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J52" s="11"/>
       <c r="AB52" s="9"/>
     </row>
-    <row r="53" spans="1:126" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B53">
         <v>-0.15</v>
@@ -4333,14 +4379,14 @@
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="I53" s="11" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="J53" s="11"/>
       <c r="AB53" s="9"/>
     </row>
-    <row r="54" spans="1:126" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B54">
         <v>0.1</v>
@@ -4349,31 +4395,31 @@
         <v>17</v>
       </c>
       <c r="I54" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="AB54" s="9"/>
     </row>
-    <row r="56" spans="1:126" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:126" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA56" s="7"/>
     </row>
-    <row r="57" spans="1:126" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>7</v>
       </c>
       <c r="B57">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H57" t="s">
         <v>17</v>
       </c>
       <c r="I57" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="58" spans="1:126" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="58" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -4381,13 +4427,13 @@
         <v>600</v>
       </c>
       <c r="H58" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="I58" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:126" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="59" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -4395,13 +4441,13 @@
         <v>20</v>
       </c>
       <c r="H59" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="I59" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="60" spans="1:126" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -4409,13 +4455,13 @@
         <v>300</v>
       </c>
       <c r="H60" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="I60" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="61" spans="1:126" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -4423,13 +4469,13 @@
         <v>970</v>
       </c>
       <c r="H61" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="I61" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="62" spans="1:126" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -4437,13 +4483,13 @@
         <v>15</v>
       </c>
       <c r="H62" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="I62" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="63" spans="1:126" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>13</v>
       </c>
@@ -4451,13 +4497,13 @@
         <v>2</v>
       </c>
       <c r="H63" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="I63" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="64" spans="1:126" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="64" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -4465,16 +4511,16 @@
         <v>380</v>
       </c>
       <c r="H64" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="I64" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="J64" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -4482,51 +4528,49 @@
         <v>209</v>
       </c>
       <c r="H65" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I65" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="67" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>34</v>
       </c>
       <c r="AA67" s="7"/>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>23</v>
       </c>
       <c r="B68">
-        <f>0.123*B51</f>
-        <v>0.246</v>
+        <v>1.79</v>
       </c>
       <c r="H68" t="s">
         <v>17</v>
       </c>
       <c r="I68" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="AB68" s="9"/>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>25</v>
       </c>
       <c r="B69">
-        <f>0.67*B51</f>
-        <v>1.34</v>
+        <v>7.6</v>
       </c>
       <c r="H69" t="s">
         <v>17</v>
       </c>
       <c r="I69" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="AB69" s="9"/>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -4534,11 +4578,11 @@
         <v>0.3</v>
       </c>
       <c r="I70" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="AB70" s="9"/>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>39</v>
       </c>
@@ -4546,14 +4590,14 @@
         <v>10</v>
       </c>
       <c r="H71" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I71" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="AB71" s="9"/>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -4561,10 +4605,10 @@
         <v>0.35</v>
       </c>
       <c r="I72" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>41</v>
       </c>
@@ -4572,10 +4616,10 @@
         <v>20.6</v>
       </c>
       <c r="I73" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>42</v>
       </c>
@@ -4583,10 +4627,10 @@
         <v>0.2</v>
       </c>
       <c r="I74" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>43</v>
       </c>
@@ -4594,10 +4638,10 @@
         <v>0.01</v>
       </c>
       <c r="I75" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>44</v>
       </c>
@@ -4605,13 +4649,13 @@
         <v>10</v>
       </c>
       <c r="H76" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I76" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>45</v>
       </c>
@@ -4619,134 +4663,134 @@
         <v>0</v>
       </c>
       <c r="H77" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="I77" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="79" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AA79" s="7"/>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>52</v>
       </c>
       <c r="B80" s="9">
-        <v>169</v>
+        <v>1.01</v>
       </c>
       <c r="I80" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="AB80" s="9"/>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>53</v>
       </c>
       <c r="B81">
-        <v>170</v>
+        <v>365.99</v>
       </c>
       <c r="I81" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="AB81" s="9"/>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>78</v>
+      </c>
+      <c r="B82">
+        <v>40.032899999999998</v>
+      </c>
+      <c r="H82" t="s">
+        <v>200</v>
+      </c>
+      <c r="I82" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB82" s="9"/>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>79</v>
       </c>
-      <c r="B82">
-        <v>52.25</v>
-      </c>
-      <c r="H82" t="s">
-        <v>206</v>
-      </c>
-      <c r="I82" t="s">
-        <v>207</v>
-      </c>
-      <c r="AB82" s="9"/>
-    </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="B83">
+        <v>254.45359999999999</v>
+      </c>
+      <c r="H83" t="s">
+        <v>200</v>
+      </c>
+      <c r="I83" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB83" s="9"/>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>80</v>
       </c>
-      <c r="B83">
-        <v>5.69</v>
-      </c>
-      <c r="H83" t="s">
-        <v>206</v>
-      </c>
-      <c r="I83" t="s">
-        <v>208</v>
-      </c>
-      <c r="AB83" s="9"/>
-    </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>81</v>
-      </c>
       <c r="B84">
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="H84" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="I84" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="86" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="AA86" s="7"/>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B87" s="9">
         <v>30</v>
       </c>
       <c r="H87" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="I87" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="AB87" s="9"/>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B88" s="9">
         <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="I88" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="AB88" s="9"/>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B89" s="9">
         <v>90</v>
       </c>
       <c r="H89" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="I89" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="AB89" s="9"/>
     </row>

</xml_diff>

<commit_message>
Added option for calculation of sun-sensor relative azimuth
Added an option to compute the relative azimuth angle (psi) within
the code, given a fixed observation azimuth angle, vazi (e.g. for a
tower-based SIF instrument facing north, vazi=180 degrees). This is
running fine BUT NOT FULLY TESTED yet.
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnorton/Models/SCOPE/SCOPE_v1.73/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD202D0-ED6A-354F-AC88-C73D6B8EE836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5385F807-3183-8A42-B269-F892FB8C6E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21160" windowHeight="15240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="349">
   <si>
     <t>Cab</t>
   </si>
@@ -306,9 +306,6 @@
     <t>leaf_file</t>
   </si>
   <si>
-    <t>FLEX-S3_std.atm</t>
-  </si>
-  <si>
     <t>year_.dat</t>
   </si>
   <si>
@@ -364,6 +361,840 @@
   </si>
   <si>
     <t>write header lines in output files</t>
+  </si>
+  <si>
+    <t>Keep the options in  this order, because Matlab reads only column A</t>
+  </si>
+  <si>
+    <t>calc_vert_profiles</t>
+  </si>
+  <si>
+    <t>calc_fluor</t>
+  </si>
+  <si>
+    <t>calc_planck</t>
+  </si>
+  <si>
+    <t>calc_directional</t>
+  </si>
+  <si>
+    <t>rt_thermal</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calculate spectrum of thermal radiation </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>with spectral emissivity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> instead of broadband</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">calculate BRDF and directional temperature for many angles specified in a file. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Be patient,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> this takes some time</t>
+    </r>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>planophile</t>
+  </si>
+  <si>
+    <t>erectophile</t>
+  </si>
+  <si>
+    <t>plagiophile</t>
+  </si>
+  <si>
+    <t>extremophile</t>
+  </si>
+  <si>
+    <t>spherical</t>
+  </si>
+  <si>
+    <t>uniform</t>
+  </si>
+  <si>
+    <t>calc_zo</t>
+  </si>
+  <si>
+    <t>0: use the zo and d values provided in the inputdata, 1: calculate zo and d from the LAI, canopy height, CD1, CR, CSSOIL (recommended if LAI changes in time series)</t>
+  </si>
+  <si>
+    <t>unit is mg m-3 in a time series file, because that is what you usually get from EC (LI7500) data</t>
+  </si>
+  <si>
+    <t>calc_rss_rbs</t>
+  </si>
+  <si>
+    <t>0: use resistance rss and rbs as provided in inputdata. 1:  calculate rss from soil moisture content and correct rbs for LAI (calc_rssrbs.m)</t>
+  </si>
+  <si>
+    <t>Fluorescence_model</t>
+  </si>
+  <si>
+    <t>0: empirical, with sustained NPQ (fit to Flexas' data); 1: empirical, with sigmoid for Kn; 2: Magnani 2012 model</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ug cm-2</t>
+  </si>
+  <si>
+    <t>Chlorophyll AB content</t>
+  </si>
+  <si>
+    <t>g cm-2</t>
+  </si>
+  <si>
+    <t>Dry matter content</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>leaf water equivalent layer</t>
+  </si>
+  <si>
+    <t>fraction</t>
+  </si>
+  <si>
+    <t>scenecent material fraction</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>leaf thickness parameters</t>
+  </si>
+  <si>
+    <t>broadband thermal reflectance</t>
+  </si>
+  <si>
+    <t>broadband thermal transmittance</t>
+  </si>
+  <si>
+    <t>umol m-2 s-1</t>
+  </si>
+  <si>
+    <t>maximum carboxylation capacity (at optimum temperature)</t>
+  </si>
+  <si>
+    <t>Ball-Berry stomatal conductance parameter</t>
+  </si>
+  <si>
+    <t>Photochemical pathway: 0=C3, 1=C4</t>
+  </si>
+  <si>
+    <t>extinction coefficient for Vcmax in the vertical (maximum at the top). 0 for uniform Vcmax</t>
+  </si>
+  <si>
+    <t>Respiration = Rdparam*Vcmcax</t>
+  </si>
+  <si>
+    <t>See PFT.xls. These are five parameters specifying the temperature response.</t>
+  </si>
+  <si>
+    <t>fluorescence quantum yield efficiency at photosystem level</t>
+  </si>
+  <si>
+    <t>Spectrum number (column in the database soil_file)</t>
+  </si>
+  <si>
+    <t>s m-1</t>
+  </si>
+  <si>
+    <t>soil resistance for evaporation from the pore space</t>
+  </si>
+  <si>
+    <t>broadband soil reflectance in the thermal range (1-emissivity)</t>
+  </si>
+  <si>
+    <t>kg m-3</t>
+  </si>
+  <si>
+    <t>specific mass of the soil</t>
+  </si>
+  <si>
+    <t>J m-1 K-1</t>
+  </si>
+  <si>
+    <t>heat conductivity of the soil</t>
+  </si>
+  <si>
+    <t>volumetric soil moisture content in the root zone</t>
+  </si>
+  <si>
+    <t>m2 m-2</t>
+  </si>
+  <si>
+    <t>Leaf area index</t>
+  </si>
+  <si>
+    <t>vegetation height</t>
+  </si>
+  <si>
+    <t>leaf inclination</t>
+  </si>
+  <si>
+    <t>variation in leaf inclination</t>
+  </si>
+  <si>
+    <t>leaf width</t>
+  </si>
+  <si>
+    <t>measurement height of meteorological data</t>
+  </si>
+  <si>
+    <t>W m-2</t>
+  </si>
+  <si>
+    <t>broadband incoming shortwave radiation (0.4-2.5 um)</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>air temperature</t>
+  </si>
+  <si>
+    <t>broadband incoming longwave radiation (2.5-50 um)</t>
+  </si>
+  <si>
+    <t>hPa</t>
+  </si>
+  <si>
+    <t>air pressure</t>
+  </si>
+  <si>
+    <t>atmospheric vapour pressure</t>
+  </si>
+  <si>
+    <t>m s-1</t>
+  </si>
+  <si>
+    <t>wind speed at height z</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>atmospheric CO2 concentration</t>
+  </si>
+  <si>
+    <t>per mille</t>
+  </si>
+  <si>
+    <t>atmospheric O2 concentration</t>
+  </si>
+  <si>
+    <t>roughness length for momentum of the canopy</t>
+  </si>
+  <si>
+    <t>displacement height</t>
+  </si>
+  <si>
+    <t>leaf drag coefficient</t>
+  </si>
+  <si>
+    <t>leaf boundary resistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verhoef et al. (1997)  Drag coefficient for isolated tree </t>
+  </si>
+  <si>
+    <t>Verhoef et al. (1997)  fitting parameter</t>
+  </si>
+  <si>
+    <t>Verhoef et al. (1997)  Roughness layer correction</t>
+  </si>
+  <si>
+    <t>Verhoef et al. (1997) Drag coefficient for soil</t>
+  </si>
+  <si>
+    <t>soil boundary layer resistance</t>
+  </si>
+  <si>
+    <t>within canopy layer resistance</t>
+  </si>
+  <si>
+    <t>Julian day (decimal) of start of simulations</t>
+  </si>
+  <si>
+    <t>Julian day (decimal) of end of simulations</t>
+  </si>
+  <si>
+    <t>decimal deg</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>east of Greenwich</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>solar zenith angle</t>
+  </si>
+  <si>
+    <t>observation zenith angle</t>
+  </si>
+  <si>
+    <t>Tyear</t>
+  </si>
+  <si>
+    <t>mean annual temperature</t>
+  </si>
+  <si>
+    <t>ºC</t>
+  </si>
+  <si>
+    <t>Leaf_Biochemical (magnani model)</t>
+  </si>
+  <si>
+    <t>fraction of photons partitioned to PSII (0.507 for C3, 0.4 for C4; Yin et al. 2006; Yin and Struik 2012)</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>rate constant of sustained thermal dissipation (Porcar-Castell 2011)</t>
+  </si>
+  <si>
+    <t>[s-1]</t>
+  </si>
+  <si>
+    <t>kNPQs</t>
+  </si>
+  <si>
+    <t>fraction of functional reaction centres (Porcar-Castell 2011)</t>
+  </si>
+  <si>
+    <t>qLs</t>
+  </si>
+  <si>
+    <t>stressfactor</t>
+  </si>
+  <si>
+    <t>optional input: stress factor to reduce Vcmax (for example soil moisture, leaf age). Default value = 1.</t>
+  </si>
+  <si>
+    <t>verifiy the results (compare to saved 'standard' output) to test the code for the first ime</t>
+  </si>
+  <si>
+    <t>In this file the input to SCOPE model (version 1.51)  is provided</t>
+  </si>
+  <si>
+    <t>The file contains the following sheets:</t>
+  </si>
+  <si>
+    <t>options: selecting optional routines for the model</t>
+  </si>
+  <si>
+    <t>filename: selecting input and output data file names</t>
+  </si>
+  <si>
+    <t>inputdata: values of the input and parameters of the model</t>
+  </si>
+  <si>
+    <t>Table 1. Example of LIDF values</t>
+  </si>
+  <si>
+    <t>Calibrated temperature sensitivity parameters for Vcmax and Resp</t>
+  </si>
+  <si>
+    <t>Field_Names</t>
+  </si>
+  <si>
+    <t>slti</t>
+  </si>
+  <si>
+    <t>shti</t>
+  </si>
+  <si>
+    <t>Thl (K)</t>
+  </si>
+  <si>
+    <t>Thh (K)</t>
+  </si>
+  <si>
+    <t>Trdm (K)</t>
+  </si>
+  <si>
+    <t>gsparam m</t>
+  </si>
+  <si>
+    <t>Respiration</t>
+  </si>
+  <si>
+    <t>Vcmax</t>
+  </si>
+  <si>
+    <t>Biome 1: Broadleaf - evergreen trees</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>Biome 2: Broadleaf - deciduous trees</t>
+  </si>
+  <si>
+    <t>Biome 3: Broadleaf and needle leaf trees</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biome 4: Needleleaf evergreen trees</t>
+  </si>
+  <si>
+    <t>Biome 5: Needleleaf deciduous trees</t>
+  </si>
+  <si>
+    <t>Biome 6: Short vegetation / C4 grassland</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Biome 7: Shrub/Stepp</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biome 8: Tree/Savanna</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Biome 9: Agriculture / C3 grassland</t>
+  </si>
+  <si>
+    <t>Shade plant</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>high light sun plant</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Desert Winter Annual</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tidestromia_Death Valley</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Table 2. Examples of biochemical parameters for the model biochemical.m</t>
+  </si>
+  <si>
+    <t>1. Introduction</t>
+  </si>
+  <si>
+    <t>This is the name of the simulation, that will also be used as output file directory</t>
+  </si>
+  <si>
+    <t>Name of a file in directory ../../data/soil_spectrum/. The first column of this file is wavelength in nm, the following columns are reflectances [0,1] of soils</t>
+  </si>
+  <si>
+    <t>Name of a file in directory ../../data/fluspect_parameters/. This files contains the Absorption Coefficients values for the FLUSPECT model</t>
+  </si>
+  <si>
+    <t>Name of a file in directory ../../data/radiationdata/. This file contains MODTRAN coefficients to calculate TOA incoming radiation</t>
+  </si>
+  <si>
+    <t>Name of a directory ../../data/input/dataset NAME/. In this folder the time series input data (below) are stored.</t>
+  </si>
+  <si>
+    <t>Name of a file containing the year numbers.</t>
+  </si>
+  <si>
+    <t>Name of file with air pressure in hPa or mbar</t>
+  </si>
+  <si>
+    <t>Name of file with value of broadband incoming shortwave radiation (0.4-3 um), in Wm-2</t>
+  </si>
+  <si>
+    <t>Name of file with value of broadband incoming longwave radiation (3-50 um) in W m-2</t>
+  </si>
+  <si>
+    <t>Name of a file containing decimal Julian day numbers (0,366), interval up to 3 hrs. The following files below have the same size as t_file.</t>
+  </si>
+  <si>
+    <t>Name of file with air temperature (in oC)</t>
+  </si>
+  <si>
+    <t>Name of file with vapour pressure (in hPa)</t>
+  </si>
+  <si>
+    <t>Name of file with ambient CO2 concentration (in mg/m3)</t>
+  </si>
+  <si>
+    <t>Name of file with wind speed (m/s)… (all at height 'z', preferably &gt;2x canopy height above the canopy)</t>
+  </si>
+  <si>
+    <t>Name of file with solar inclination in deg. If this is not provided, then solar inclination is calculated from LAT, LON and DOY.</t>
+  </si>
+  <si>
+    <t>The following fiels have two columns: one with DOY (can be different for each file, and different from the values in t_file) and one with values of height (in m).</t>
+  </si>
+  <si>
+    <t>The values in the file are linearly interpolated to those in t_file!</t>
+  </si>
+  <si>
+    <t>Name of file with single sided Leaf Area Index (m2/m2)</t>
+  </si>
+  <si>
+    <t>Name of file with vegetation height (m)</t>
+  </si>
+  <si>
+    <t>name of file with maximum carboxylation capacity (umol m-2 s-1)</t>
+  </si>
+  <si>
+    <t>Name of file with chlorophyll concentrations (mg cm-2)</t>
+  </si>
+  <si>
+    <t>Name of file with the height of measurements (m).</t>
+  </si>
+  <si>
+    <t>If (some of) these files are not provided, then the values in the inputdata tab are used.</t>
+  </si>
+  <si>
+    <t>This file will be saved along with the simulation output</t>
+  </si>
+  <si>
+    <t>readme: explanation for the user (this sheet is ignored by the model code)</t>
+  </si>
+  <si>
+    <t>2. Tab options</t>
+  </si>
+  <si>
+    <t>See the comments in the tab for explanation of the options</t>
+  </si>
+  <si>
+    <t>3. Tab filenames</t>
+  </si>
+  <si>
+    <t>4. Tab inputdata</t>
+  </si>
+  <si>
+    <t>See explanation and units of the variables in the tab inputdata itself.</t>
+  </si>
+  <si>
+    <t>Some reference values for parameters: see tables below</t>
+  </si>
+  <si>
+    <t>name of file with soil moisture content values (volumetric fraction) in the top soil (0-5 cm), only used for soil heat flux at the moment</t>
+  </si>
+  <si>
+    <t>Table 3. Typical ranges of input values</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Air pressure</t>
+  </si>
+  <si>
+    <t>Oxygen pressure</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Dark respiration coefficient</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <t>umol m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> s</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[CO2]</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>L</t>
+    </r>
+  </si>
+  <si>
+    <t>Photosynthetic capacity</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>cmo</t>
+    </r>
+  </si>
+  <si>
+    <t>Stress multiplier for Vcmo</t>
+  </si>
+  <si>
+    <t>Stressfactor</t>
+  </si>
+  <si>
+    <t>Rate thermal dissipation</t>
+  </si>
+  <si>
+    <t>Fraction active photosystems</t>
+  </si>
+  <si>
+    <t>Vapour pressure</t>
+  </si>
+  <si>
+    <t>typical value</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ball Berry Stomatal param </t>
+  </si>
+  <si>
+    <t>0.7*satvap(Ta)</t>
+  </si>
+  <si>
+    <t>0.1*satvap(Ta)</t>
+  </si>
+  <si>
+    <t>1.0*satvap(Ta)</t>
+  </si>
+  <si>
+    <t>CO2 concentration</t>
+  </si>
+  <si>
+    <t>80 (C3) ,30 (C4)</t>
+  </si>
+  <si>
+    <t>Cca</t>
+  </si>
+  <si>
+    <t>Carotenoid content. Usually 25% of Cab</t>
+  </si>
+  <si>
+    <t>soil_heat_method</t>
+  </si>
+  <si>
+    <t>save_headers</t>
+  </si>
+  <si>
+    <t>apply_T_corr</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The order of the parameters is not relevant, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>but the names of the variables should not be changed</t>
+    </r>
+  </si>
+  <si>
+    <t>specific heat capacity of the soil</t>
+  </si>
+  <si>
+    <t>J kg-1 K-1</t>
+  </si>
+  <si>
+    <t>calc_xanthophyllabs</t>
+  </si>
+  <si>
+    <t>BallBerry0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cant </t>
+  </si>
+  <si>
+    <t>Anthocyanins</t>
+  </si>
+  <si>
+    <t>Optipar2017_ProspectD.mat</t>
+  </si>
+  <si>
+    <t>0 (recommended): treat the whole fluorescence spectrum as one spectrum (new calibrated optipar), 1: differentiate PSI and PSII with Franck et al. spectra (of SCOPE 1.62 and older)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calc_PSI      </t>
+  </si>
+  <si>
+    <t>calculate dynamic xanthopyll absorption (zeaxanthin), for simulating PRI</t>
+  </si>
+  <si>
+    <t>soilspectrum</t>
+  </si>
+  <si>
+    <t>0: use soil spectrum from a file, 1: simulate soil spectrum with the BSM model</t>
+  </si>
+  <si>
+    <t>BSMlat</t>
+  </si>
+  <si>
+    <t>BSMlon</t>
+  </si>
+  <si>
+    <t>BSM model parameter for soil brightness</t>
+  </si>
+  <si>
+    <t>BSM model parameter 'lat'</t>
+  </si>
+  <si>
+    <t>BSM model parameter  'long'</t>
+  </si>
+  <si>
+    <t>BSMBrightness</t>
+  </si>
+  <si>
+    <t>LIDF_file</t>
+  </si>
+  <si>
+    <t>optiona_leaf_inclination_distribution_file_with_3_headerlines._MUST_be_located_in_../data/leafangles/</t>
+  </si>
+  <si>
+    <t>optional_(leave_empty_for_calculations_based_on_t_file_year_timezn)</t>
+  </si>
+  <si>
+    <t>doy_.dat</t>
+  </si>
+  <si>
+    <t>sw_.dat</t>
+  </si>
+  <si>
+    <t>lw_.dat</t>
+  </si>
+  <si>
+    <t>ps_.dat</t>
+  </si>
+  <si>
+    <t>ta_.dat</t>
+  </si>
+  <si>
+    <t>lai_constant_.dat</t>
+  </si>
+  <si>
+    <t>CA-OBS-2019</t>
+  </si>
+  <si>
+    <t>calculate the azimuthal difference between solar and observation angle (psi) according to a fixed observation azimuth angle (i.e. psi varies according to the sun-sensor geometry)</t>
+  </si>
+  <si>
+    <t>dynamic_azimuth</t>
+  </si>
+  <si>
+    <t>vazi</t>
+  </si>
+  <si>
+    <t>fixed point observation azimuth angle e.g. 180=North (only used if options.dynamic_azimuth = 1)</t>
+  </si>
+  <si>
+    <t>azimuthal difference between solar and observation angle  (not used if options.dynamic_azimuth = 1 and options.simulation = 1)</t>
+  </si>
+  <si>
+    <t>FLEX-S3_V80.atm</t>
   </si>
   <si>
     <r>
@@ -407,877 +1238,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>of values for all input that varies between the runs.</t>
+      <t>of values for all input that varies between the runs. 1: time series (uses text files with meteo input as time series). 2: Lookup-Table (specify the values to be included. All possible combinations of inputs will be  used)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>2: Lookup-Table (specify the values to be included.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> All possible combinations </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>of inputs will be  used)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1: time series (uses </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">text files </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>with meteo input as time series)</t>
-    </r>
-  </si>
-  <si>
-    <t>Keep the options in  this order, because Matlab reads only column A</t>
-  </si>
-  <si>
-    <t>calc_vert_profiles</t>
-  </si>
-  <si>
-    <t>calc_fluor</t>
-  </si>
-  <si>
-    <t>calc_planck</t>
-  </si>
-  <si>
-    <t>calc_directional</t>
-  </si>
-  <si>
-    <t>rt_thermal</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">calculate spectrum of thermal radiation </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>with spectral emissivity</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> instead of broadband</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">calculate BRDF and directional temperature for many angles specified in a file. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Be patient,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> this takes some time</t>
-    </r>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>planophile</t>
-  </si>
-  <si>
-    <t>erectophile</t>
-  </si>
-  <si>
-    <t>plagiophile</t>
-  </si>
-  <si>
-    <t>extremophile</t>
-  </si>
-  <si>
-    <t>spherical</t>
-  </si>
-  <si>
-    <t>uniform</t>
-  </si>
-  <si>
-    <t>calc_zo</t>
-  </si>
-  <si>
-    <t>0: use the zo and d values provided in the inputdata, 1: calculate zo and d from the LAI, canopy height, CD1, CR, CSSOIL (recommended if LAI changes in time series)</t>
-  </si>
-  <si>
-    <t>unit is mg m-3 in a time series file, because that is what you usually get from EC (LI7500) data</t>
-  </si>
-  <si>
-    <t>calc_rss_rbs</t>
-  </si>
-  <si>
-    <t>0: use resistance rss and rbs as provided in inputdata. 1:  calculate rss from soil moisture content and correct rbs for LAI (calc_rssrbs.m)</t>
-  </si>
-  <si>
-    <t>Fluorescence_model</t>
-  </si>
-  <si>
-    <t>0: empirical, with sustained NPQ (fit to Flexas' data); 1: empirical, with sigmoid for Kn; 2: Magnani 2012 model</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>ug cm-2</t>
-  </si>
-  <si>
-    <t>Chlorophyll AB content</t>
-  </si>
-  <si>
-    <t>g cm-2</t>
-  </si>
-  <si>
-    <t>Dry matter content</t>
-  </si>
-  <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>leaf water equivalent layer</t>
-  </si>
-  <si>
-    <t>fraction</t>
-  </si>
-  <si>
-    <t>scenecent material fraction</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>leaf thickness parameters</t>
-  </si>
-  <si>
-    <t>broadband thermal reflectance</t>
-  </si>
-  <si>
-    <t>broadband thermal transmittance</t>
-  </si>
-  <si>
-    <t>umol m-2 s-1</t>
-  </si>
-  <si>
-    <t>maximum carboxylation capacity (at optimum temperature)</t>
-  </si>
-  <si>
-    <t>Ball-Berry stomatal conductance parameter</t>
-  </si>
-  <si>
-    <t>Photochemical pathway: 0=C3, 1=C4</t>
-  </si>
-  <si>
-    <t>extinction coefficient for Vcmax in the vertical (maximum at the top). 0 for uniform Vcmax</t>
-  </si>
-  <si>
-    <t>Respiration = Rdparam*Vcmcax</t>
-  </si>
-  <si>
-    <t>See PFT.xls. These are five parameters specifying the temperature response.</t>
-  </si>
-  <si>
-    <t>fluorescence quantum yield efficiency at photosystem level</t>
-  </si>
-  <si>
-    <t>Spectrum number (column in the database soil_file)</t>
-  </si>
-  <si>
-    <t>s m-1</t>
-  </si>
-  <si>
-    <t>soil resistance for evaporation from the pore space</t>
-  </si>
-  <si>
-    <t>broadband soil reflectance in the thermal range (1-emissivity)</t>
-  </si>
-  <si>
-    <t>kg m-3</t>
-  </si>
-  <si>
-    <t>specific mass of the soil</t>
-  </si>
-  <si>
-    <t>J m-1 K-1</t>
-  </si>
-  <si>
-    <t>heat conductivity of the soil</t>
-  </si>
-  <si>
-    <t>volumetric soil moisture content in the root zone</t>
-  </si>
-  <si>
-    <t>m2 m-2</t>
-  </si>
-  <si>
-    <t>Leaf area index</t>
-  </si>
-  <si>
-    <t>vegetation height</t>
-  </si>
-  <si>
-    <t>leaf inclination</t>
-  </si>
-  <si>
-    <t>variation in leaf inclination</t>
-  </si>
-  <si>
-    <t>leaf width</t>
-  </si>
-  <si>
-    <t>measurement height of meteorological data</t>
-  </si>
-  <si>
-    <t>W m-2</t>
-  </si>
-  <si>
-    <t>broadband incoming shortwave radiation (0.4-2.5 um)</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>air temperature</t>
-  </si>
-  <si>
-    <t>broadband incoming longwave radiation (2.5-50 um)</t>
-  </si>
-  <si>
-    <t>hPa</t>
-  </si>
-  <si>
-    <t>air pressure</t>
-  </si>
-  <si>
-    <t>atmospheric vapour pressure</t>
-  </si>
-  <si>
-    <t>m s-1</t>
-  </si>
-  <si>
-    <t>wind speed at height z</t>
-  </si>
-  <si>
-    <t>ppm</t>
-  </si>
-  <si>
-    <t>atmospheric CO2 concentration</t>
-  </si>
-  <si>
-    <t>per mille</t>
-  </si>
-  <si>
-    <t>atmospheric O2 concentration</t>
-  </si>
-  <si>
-    <t>roughness length for momentum of the canopy</t>
-  </si>
-  <si>
-    <t>displacement height</t>
-  </si>
-  <si>
-    <t>leaf drag coefficient</t>
-  </si>
-  <si>
-    <t>leaf boundary resistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verhoef et al. (1997)  Drag coefficient for isolated tree </t>
-  </si>
-  <si>
-    <t>Verhoef et al. (1997)  fitting parameter</t>
-  </si>
-  <si>
-    <t>Verhoef et al. (1997)  Roughness layer correction</t>
-  </si>
-  <si>
-    <t>Verhoef et al. (1997) Drag coefficient for soil</t>
-  </si>
-  <si>
-    <t>soil boundary layer resistance</t>
-  </si>
-  <si>
-    <t>within canopy layer resistance</t>
-  </si>
-  <si>
-    <t>Julian day (decimal) of start of simulations</t>
-  </si>
-  <si>
-    <t>Julian day (decimal) of end of simulations</t>
-  </si>
-  <si>
-    <t>decimal deg</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>hours</t>
-  </si>
-  <si>
-    <t>east of Greenwich</t>
-  </si>
-  <si>
-    <t>deg</t>
-  </si>
-  <si>
-    <t>solar zenith angle</t>
-  </si>
-  <si>
-    <t>observation zenith angle</t>
-  </si>
-  <si>
-    <t>azimuthal difference between solar and observation angle</t>
-  </si>
-  <si>
-    <t>Tyear</t>
-  </si>
-  <si>
-    <t>mean annual temperature</t>
-  </si>
-  <si>
-    <t>ºC</t>
-  </si>
-  <si>
-    <t>Leaf_Biochemical (magnani model)</t>
-  </si>
-  <si>
-    <t>fraction of photons partitioned to PSII (0.507 for C3, 0.4 for C4; Yin et al. 2006; Yin and Struik 2012)</t>
-  </si>
-  <si>
-    <t>beta</t>
-  </si>
-  <si>
-    <t>rate constant of sustained thermal dissipation (Porcar-Castell 2011)</t>
-  </si>
-  <si>
-    <t>[s-1]</t>
-  </si>
-  <si>
-    <t>kNPQs</t>
-  </si>
-  <si>
-    <t>fraction of functional reaction centres (Porcar-Castell 2011)</t>
-  </si>
-  <si>
-    <t>qLs</t>
-  </si>
-  <si>
-    <t>stressfactor</t>
-  </si>
-  <si>
-    <t>optional input: stress factor to reduce Vcmax (for example soil moisture, leaf age). Default value = 1.</t>
-  </si>
-  <si>
-    <t>verifiy the results (compare to saved 'standard' output) to test the code for the first ime</t>
-  </si>
-  <si>
-    <t>In this file the input to SCOPE model (version 1.51)  is provided</t>
-  </si>
-  <si>
-    <t>The file contains the following sheets:</t>
-  </si>
-  <si>
-    <t>options: selecting optional routines for the model</t>
-  </si>
-  <si>
-    <t>filename: selecting input and output data file names</t>
-  </si>
-  <si>
-    <t>inputdata: values of the input and parameters of the model</t>
-  </si>
-  <si>
-    <t>Table 1. Example of LIDF values</t>
-  </si>
-  <si>
-    <t>Calibrated temperature sensitivity parameters for Vcmax and Resp</t>
-  </si>
-  <si>
-    <t>Field_Names</t>
-  </si>
-  <si>
-    <t>slti</t>
-  </si>
-  <si>
-    <t>shti</t>
-  </si>
-  <si>
-    <t>Thl (K)</t>
-  </si>
-  <si>
-    <t>Thh (K)</t>
-  </si>
-  <si>
-    <t>Trdm (K)</t>
-  </si>
-  <si>
-    <t>gsparam m</t>
-  </si>
-  <si>
-    <t>Respiration</t>
-  </si>
-  <si>
-    <t>Vcmax</t>
-  </si>
-  <si>
-    <t>Biome 1: Broadleaf - evergreen trees</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>Biome 2: Broadleaf - deciduous trees</t>
-  </si>
-  <si>
-    <t>Biome 3: Broadleaf and needle leaf trees</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biome 4: Needleleaf evergreen trees</t>
-  </si>
-  <si>
-    <t>Biome 5: Needleleaf deciduous trees</t>
-  </si>
-  <si>
-    <t>Biome 6: Short vegetation / C4 grassland</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>Biome 7: Shrub/Stepp</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biome 8: Tree/Savanna</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biome 9: Agriculture / C3 grassland</t>
-  </si>
-  <si>
-    <t>Shade plant</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>high light sun plant</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Desert Winter Annual</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tidestromia_Death Valley</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Table 2. Examples of biochemical parameters for the model biochemical.m</t>
-  </si>
-  <si>
-    <t>1. Introduction</t>
-  </si>
-  <si>
-    <t>This is the name of the simulation, that will also be used as output file directory</t>
-  </si>
-  <si>
-    <t>Name of a file in directory ../../data/soil_spectrum/. The first column of this file is wavelength in nm, the following columns are reflectances [0,1] of soils</t>
-  </si>
-  <si>
-    <t>Name of a file in directory ../../data/fluspect_parameters/. This files contains the Absorption Coefficients values for the FLUSPECT model</t>
-  </si>
-  <si>
-    <t>Name of a file in directory ../../data/radiationdata/. This file contains MODTRAN coefficients to calculate TOA incoming radiation</t>
-  </si>
-  <si>
-    <t>Name of a directory ../../data/input/dataset NAME/. In this folder the time series input data (below) are stored.</t>
-  </si>
-  <si>
-    <t>Name of a file containing the year numbers.</t>
-  </si>
-  <si>
-    <t>Name of file with air pressure in hPa or mbar</t>
-  </si>
-  <si>
-    <t>Name of file with value of broadband incoming shortwave radiation (0.4-3 um), in Wm-2</t>
-  </si>
-  <si>
-    <t>Name of file with value of broadband incoming longwave radiation (3-50 um) in W m-2</t>
-  </si>
-  <si>
-    <t>Name of a file containing decimal Julian day numbers (0,366), interval up to 3 hrs. The following files below have the same size as t_file.</t>
-  </si>
-  <si>
-    <t>Name of file with air temperature (in oC)</t>
-  </si>
-  <si>
-    <t>Name of file with vapour pressure (in hPa)</t>
-  </si>
-  <si>
-    <t>Name of file with ambient CO2 concentration (in mg/m3)</t>
-  </si>
-  <si>
-    <t>Name of file with wind speed (m/s)… (all at height 'z', preferably &gt;2x canopy height above the canopy)</t>
-  </si>
-  <si>
-    <t>Name of file with solar inclination in deg. If this is not provided, then solar inclination is calculated from LAT, LON and DOY.</t>
-  </si>
-  <si>
-    <t>The following fiels have two columns: one with DOY (can be different for each file, and different from the values in t_file) and one with values of height (in m).</t>
-  </si>
-  <si>
-    <t>The values in the file are linearly interpolated to those in t_file!</t>
-  </si>
-  <si>
-    <t>Name of file with single sided Leaf Area Index (m2/m2)</t>
-  </si>
-  <si>
-    <t>Name of file with vegetation height (m)</t>
-  </si>
-  <si>
-    <t>name of file with maximum carboxylation capacity (umol m-2 s-1)</t>
-  </si>
-  <si>
-    <t>Name of file with chlorophyll concentrations (mg cm-2)</t>
-  </si>
-  <si>
-    <t>Name of file with the height of measurements (m).</t>
-  </si>
-  <si>
-    <t>If (some of) these files are not provided, then the values in the inputdata tab are used.</t>
-  </si>
-  <si>
-    <t>This file will be saved along with the simulation output</t>
-  </si>
-  <si>
-    <t>readme: explanation for the user (this sheet is ignored by the model code)</t>
-  </si>
-  <si>
-    <t>2. Tab options</t>
-  </si>
-  <si>
-    <t>See the comments in the tab for explanation of the options</t>
-  </si>
-  <si>
-    <t>3. Tab filenames</t>
-  </si>
-  <si>
-    <t>4. Tab inputdata</t>
-  </si>
-  <si>
-    <t>See explanation and units of the variables in the tab inputdata itself.</t>
-  </si>
-  <si>
-    <t>Some reference values for parameters: see tables below</t>
-  </si>
-  <si>
-    <t>name of file with soil moisture content values (volumetric fraction) in the top soil (0-5 cm), only used for soil heat flux at the moment</t>
-  </si>
-  <si>
-    <t>Table 3. Typical ranges of input values</t>
-  </si>
-  <si>
-    <t>Symbol</t>
-  </si>
-  <si>
-    <t>Air pressure</t>
-  </si>
-  <si>
-    <t>Oxygen pressure</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>Dark respiration coefficient</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <r>
-      <t>umol m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> s</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[CO2]</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>L</t>
-    </r>
-  </si>
-  <si>
-    <t>Photosynthetic capacity</t>
-  </si>
-  <si>
-    <r>
-      <t>V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>cmo</t>
-    </r>
-  </si>
-  <si>
-    <t>Stress multiplier for Vcmo</t>
-  </si>
-  <si>
-    <t>Stressfactor</t>
-  </si>
-  <si>
-    <t>Rate thermal dissipation</t>
-  </si>
-  <si>
-    <t>Fraction active photosystems</t>
-  </si>
-  <si>
-    <t>Vapour pressure</t>
-  </si>
-  <si>
-    <t>typical value</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ball Berry Stomatal param </t>
-  </si>
-  <si>
-    <t>0.7*satvap(Ta)</t>
-  </si>
-  <si>
-    <t>0.1*satvap(Ta)</t>
-  </si>
-  <si>
-    <t>1.0*satvap(Ta)</t>
-  </si>
-  <si>
-    <t>CO2 concentration</t>
-  </si>
-  <si>
-    <t>80 (C3) ,30 (C4)</t>
-  </si>
-  <si>
-    <t>Cca</t>
-  </si>
-  <si>
-    <t>Carotenoid content. Usually 25% of Cab</t>
-  </si>
-  <si>
-    <t>soil_heat_method</t>
-  </si>
-  <si>
-    <t>save_headers</t>
-  </si>
-  <si>
-    <t>apply_T_corr</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The order of the parameters is not relevant, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>but the names of the variables should not be changed</t>
-    </r>
-  </si>
-  <si>
-    <t>specific heat capacity of the soil</t>
-  </si>
-  <si>
-    <t>J kg-1 K-1</t>
-  </si>
-  <si>
-    <t>calc_xanthophyllabs</t>
-  </si>
-  <si>
-    <t>BallBerry0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cant </t>
-  </si>
-  <si>
-    <t>Anthocyanins</t>
-  </si>
-  <si>
-    <t>Optipar2017_ProspectD.mat</t>
-  </si>
-  <si>
-    <t>0 (recommended): treat the whole fluorescence spectrum as one spectrum (new calibrated optipar), 1: differentiate PSI and PSII with Franck et al. spectra (of SCOPE 1.62 and older)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calc_PSI      </t>
-  </si>
-  <si>
-    <t>calculate dynamic xanthopyll absorption (zeaxanthin), for simulating PRI</t>
-  </si>
-  <si>
-    <t>soilspectrum</t>
-  </si>
-  <si>
-    <t>0: use soil spectrum from a file, 1: simulate soil spectrum with the BSM model</t>
-  </si>
-  <si>
-    <t>BSMlat</t>
-  </si>
-  <si>
-    <t>BSMlon</t>
-  </si>
-  <si>
-    <t>BSM model parameter for soil brightness</t>
-  </si>
-  <si>
-    <t>BSM model parameter 'lat'</t>
-  </si>
-  <si>
-    <t>BSM model parameter  'long'</t>
-  </si>
-  <si>
-    <t>BSMBrightness</t>
-  </si>
-  <si>
-    <t>LIDF_file</t>
-  </si>
-  <si>
-    <t>optiona_leaf_inclination_distribution_file_with_3_headerlines._MUST_be_located_in_../data/leafangles/</t>
-  </si>
-  <si>
-    <t>optional_(leave_empty_for_calculations_based_on_t_file_year_timezn)</t>
-  </si>
-  <si>
-    <t>doy_.dat</t>
-  </si>
-  <si>
-    <t>sw_.dat</t>
-  </si>
-  <si>
-    <t>lw_.dat</t>
-  </si>
-  <si>
-    <t>ps_.dat</t>
-  </si>
-  <si>
-    <t>ta_.dat</t>
-  </si>
-  <si>
-    <t>lai_constant_.dat</t>
-  </si>
-  <si>
-    <t>US-NR1-2017</t>
   </si>
 </sst>
 </file>
@@ -1621,7 +1583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1720,6 +1682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2069,7 +2032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J96"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2089,57 +2052,57 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="38" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="37" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2147,7 +2110,7 @@
         <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2155,7 +2118,7 @@
         <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2163,7 +2126,7 @@
         <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2171,7 +2134,7 @@
         <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2184,7 +2147,7 @@
         <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2192,7 +2155,7 @@
         <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2200,7 +2163,7 @@
         <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2208,7 +2171,7 @@
         <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2216,7 +2179,7 @@
         <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2224,7 +2187,7 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2232,7 +2195,7 @@
         <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2240,7 +2203,7 @@
         <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2248,12 +2211,12 @@
         <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2261,7 +2224,7 @@
         <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2269,7 +2232,7 @@
         <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2280,17 +2243,17 @@
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="C39" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2298,7 +2261,7 @@
         <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2306,7 +2269,7 @@
         <v>69</v>
       </c>
       <c r="C43" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2314,7 +2277,7 @@
         <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2322,7 +2285,7 @@
         <v>71</v>
       </c>
       <c r="C45" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2330,7 +2293,7 @@
         <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2338,48 +2301,48 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="37" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="36" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="52" t="s">
-        <v>122</v>
-      </c>
-      <c r="B56" s="52" t="s">
+      <c r="A56" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="C56" s="52" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="57" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="53"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="53"/>
+      <c r="A57" s="54"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="54"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B58" s="11">
         <v>1</v>
@@ -2390,7 +2353,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B59" s="11">
         <v>-1</v>
@@ -2401,7 +2364,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B60" s="11">
         <v>0</v>
@@ -2412,7 +2375,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B61" s="11">
         <v>0</v>
@@ -2423,7 +2386,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B62" s="11">
         <v>-0.35</v>
@@ -2434,7 +2397,7 @@
     </row>
     <row r="63" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B63" s="12">
         <v>0</v>
@@ -2445,61 +2408,61 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="36" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="15"/>
       <c r="B68" s="16"/>
-      <c r="C68" s="54" t="s">
-        <v>229</v>
-      </c>
-      <c r="D68" s="55"/>
-      <c r="E68" s="55"/>
-      <c r="F68" s="55"/>
-      <c r="G68" s="56"/>
+      <c r="C68" s="55" t="s">
+        <v>224</v>
+      </c>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
+      <c r="G68" s="57"/>
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
       <c r="J68" s="18"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B69" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C69" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="D69" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="G69" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="H69" s="22" t="s">
         <v>231</v>
       </c>
-      <c r="D69" s="22" t="s">
+      <c r="I69" s="22" t="s">
         <v>232</v>
       </c>
-      <c r="E69" s="22" t="s">
+      <c r="J69" s="23" t="s">
         <v>233</v>
-      </c>
-      <c r="F69" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="G69" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="H69" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="I69" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="J69" s="23" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="24" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C70" s="25">
         <v>0.2</v>
@@ -2528,10 +2491,10 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="24" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C71" s="25">
         <v>0.2</v>
@@ -2560,10 +2523,10 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C72" s="25">
         <v>0.2</v>
@@ -2592,10 +2555,10 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C73" s="25">
         <v>0.2</v>
@@ -2624,10 +2587,10 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="24" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C74" s="25">
         <v>0.2</v>
@@ -2656,10 +2619,10 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="24" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C75" s="25">
         <v>0.2</v>
@@ -2688,10 +2651,10 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="24" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C76" s="25">
         <v>0.2</v>
@@ -2720,10 +2683,10 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="24" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C77" s="25">
         <v>0.2</v>
@@ -2752,10 +2715,10 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="24" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C78" s="25">
         <v>0.2</v>
@@ -2784,10 +2747,10 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="24" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C79" s="25">
         <v>0.2</v>
@@ -2816,10 +2779,10 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="24" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C80" s="25">
         <v>0.2</v>
@@ -2848,10 +2811,10 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="24" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C81" s="25">
         <v>0.2</v>
@@ -2880,10 +2843,10 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="31" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B82" s="32" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C82" s="33">
         <v>0.2</v>
@@ -2912,7 +2875,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="36" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
@@ -2920,30 +2883,30 @@
         <v>74</v>
       </c>
       <c r="B86" s="41" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C86" s="41" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D86" s="41" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E86" s="41" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F86" s="41" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="39" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B87" s="39" t="s">
         <v>11</v>
       </c>
       <c r="C87" s="39" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D87" s="42">
         <v>1000</v>
@@ -2958,13 +2921,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="39" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B88" s="39" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C88" s="39" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D88" s="42">
         <v>209</v>
@@ -2979,13 +2942,13 @@
     </row>
     <row r="89" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A89" s="39" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B89" s="39" t="s">
         <v>21</v>
       </c>
       <c r="C89" s="39" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D89" s="43">
         <v>1.4999999999999999E-2</v>
@@ -3000,13 +2963,13 @@
     </row>
     <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A90" s="39" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B90" s="39" t="s">
         <v>17</v>
       </c>
       <c r="C90" s="39" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D90" s="43">
         <v>7</v>
@@ -3021,34 +2984,34 @@
     </row>
     <row r="91" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="39" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B91" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C91" s="39" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D91" s="42" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E91" s="42" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F91" s="42" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="G91" s="42"/>
     </row>
     <row r="92" spans="1:10" ht="19" x14ac:dyDescent="0.2">
       <c r="A92" s="39" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B92" s="39" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C92" s="39" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D92" s="42">
         <v>380</v>
@@ -3062,16 +3025,16 @@
     </row>
     <row r="93" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A93" s="39" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B93" s="40" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C93" s="39" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D93" s="42" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E93" s="42">
         <v>0</v>
@@ -3082,13 +3045,13 @@
     </row>
     <row r="94" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A94" s="39" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B94" s="39" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C94" s="39" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D94" s="42">
         <v>1</v>
@@ -3102,13 +3065,13 @@
     </row>
     <row r="95" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A95" s="44" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B95" s="44" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C95" s="44" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D95" s="45">
         <v>0</v>
@@ -3122,13 +3085,13 @@
     </row>
     <row r="96" spans="1:10" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A96" s="46" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B96" s="46" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C96" s="46" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D96" s="47">
         <v>1</v>
@@ -3155,10 +3118,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3174,7 +3137,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3196,10 +3159,10 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3207,10 +3170,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -3218,10 +3181,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3229,10 +3192,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3240,10 +3203,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E10" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -3251,10 +3214,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E11" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3262,10 +3225,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3273,10 +3236,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -3284,10 +3247,10 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E14" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3295,10 +3258,10 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3306,10 +3269,10 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E16" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3317,10 +3280,10 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3328,7 +3291,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E18" t="s">
         <v>48</v>
@@ -3342,7 +3305,7 @@
         <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3350,15 +3313,15 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
@@ -3375,18 +3338,18 @@
         <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>348</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
+      <c r="A23" s="52">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>343</v>
+      </c>
       <c r="E23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E24" t="s">
-        <v>112</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -3401,7 +3364,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3427,7 +3390,7 @@
         <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3435,7 +3398,7 @@
         <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3443,7 +3406,7 @@
         <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3451,7 +3414,7 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3464,7 +3427,7 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3472,7 +3435,7 @@
         <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3480,7 +3443,7 @@
         <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3488,7 +3451,7 @@
         <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3496,7 +3459,7 @@
         <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3504,7 +3467,7 @@
         <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3512,7 +3475,7 @@
         <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -3520,7 +3483,7 @@
         <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3528,12 +3491,12 @@
         <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3548,7 +3511,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="51" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -3571,7 +3534,7 @@
         <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -3591,12 +3554,12 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="50" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
@@ -3611,10 +3574,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:DV89"/>
+  <dimension ref="A1:DV90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3634,7 +3597,7 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -3650,10 +3613,10 @@
         <v>75</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="AA6" s="8"/>
       <c r="AB6" s="5"/>
@@ -3672,25 +3635,25 @@
         <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I9" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="AA9"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B10">
         <v>6.25</v>
       </c>
       <c r="H10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I10" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="AA10"/>
     </row>
@@ -3702,10 +3665,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="H11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="AA11"/>
     </row>
@@ -3717,10 +3680,10 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="H12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="AA12"/>
     </row>
@@ -3732,25 +3695,25 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="AA13"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I14" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="AA14"/>
     </row>
@@ -3762,10 +3725,10 @@
         <v>1.4</v>
       </c>
       <c r="H15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="AA15"/>
     </row>
@@ -3778,7 +3741,7 @@
       </c>
       <c r="E16" s="13"/>
       <c r="I16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AA16"/>
     </row>
@@ -3790,7 +3753,7 @@
         <v>0.01</v>
       </c>
       <c r="I17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="AA17"/>
     </row>
@@ -3799,7 +3762,7 @@
     </row>
     <row r="19" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:103" x14ac:dyDescent="0.2">
@@ -3807,13 +3770,13 @@
         <v>16</v>
       </c>
       <c r="B20">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H20" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="AA20"/>
     </row>
@@ -3825,7 +3788,7 @@
         <v>8</v>
       </c>
       <c r="I21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="AB21" s="9"/>
       <c r="AZ21" s="4"/>
@@ -3837,7 +3800,7 @@
     </row>
     <row r="22" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3858,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="AB23" s="9"/>
       <c r="AZ23" s="4"/>
@@ -3876,7 +3839,7 @@
         <v>0.63959999999999995</v>
       </c>
       <c r="I24" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="AA24"/>
     </row>
@@ -3888,7 +3851,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I25" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="AB25" s="9"/>
       <c r="AZ25" s="4"/>
@@ -3918,7 +3881,7 @@
         <v>328</v>
       </c>
       <c r="I26" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="AZ26" s="4"/>
       <c r="BY26" s="4"/>
@@ -3926,21 +3889,21 @@
     </row>
     <row r="27" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B28">
         <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I28" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="AZ28" s="4"/>
       <c r="BY28" s="4"/>
@@ -3948,16 +3911,16 @@
     </row>
     <row r="29" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B29">
         <v>0.50700000000000001</v>
       </c>
       <c r="H29" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I29" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="AZ29" s="4"/>
       <c r="BY29" s="4"/>
@@ -3965,16 +3928,16 @@
     </row>
     <row r="30" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I30" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="AZ30" s="4"/>
       <c r="BY30" s="4"/>
@@ -3982,16 +3945,16 @@
     </row>
     <row r="31" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I31" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="AZ31" s="4"/>
       <c r="BY31" s="4"/>
@@ -3999,13 +3962,13 @@
     </row>
     <row r="32" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="AZ32" s="4"/>
       <c r="BY32" s="4"/>
@@ -4034,7 +3997,7 @@
       </c>
       <c r="G35" s="13"/>
       <c r="I35" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="AB35" s="9"/>
       <c r="AZ35" s="4"/>
@@ -4066,7 +4029,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="AZ38" s="4"/>
       <c r="BY38" s="4"/>
@@ -4080,10 +4043,10 @@
         <v>500</v>
       </c>
       <c r="H39" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I39" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AZ39" s="4"/>
       <c r="BY39" s="4"/>
@@ -4097,7 +4060,7 @@
         <v>0.06</v>
       </c>
       <c r="I40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="AZ40" s="4"/>
       <c r="BY40" s="4"/>
@@ -4111,10 +4074,10 @@
         <v>1180</v>
       </c>
       <c r="H41" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I41" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="AZ41" s="4"/>
       <c r="BY41" s="4"/>
@@ -4128,10 +4091,10 @@
         <v>1800</v>
       </c>
       <c r="H42" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I42" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="AZ42" s="4"/>
       <c r="BY42" s="4"/>
@@ -4145,10 +4108,10 @@
         <v>1.55</v>
       </c>
       <c r="H43" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I43" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="AZ43" s="4"/>
       <c r="BY43" s="4"/>
@@ -4156,13 +4119,13 @@
     </row>
     <row r="44" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B44">
         <v>0.5</v>
       </c>
       <c r="I44" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="AZ44" s="4"/>
       <c r="BY44" s="4"/>
@@ -4170,13 +4133,13 @@
     </row>
     <row r="45" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B45">
         <v>0.5</v>
       </c>
       <c r="I45" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="AZ45" s="4"/>
       <c r="BY45" s="4"/>
@@ -4184,13 +4147,13 @@
     </row>
     <row r="46" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B46">
         <v>25</v>
       </c>
       <c r="I46" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="AZ46" s="4"/>
       <c r="BY46" s="4"/>
@@ -4198,13 +4161,13 @@
     </row>
     <row r="47" spans="1:103" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B47">
         <v>45</v>
       </c>
       <c r="I47" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="AZ47" s="4"/>
       <c r="BY47" s="4"/>
@@ -4232,10 +4195,10 @@
         <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I50" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="AB50" s="4"/>
       <c r="AC50" s="4"/>
@@ -4348,13 +4311,13 @@
         <v>17</v>
       </c>
       <c r="I51" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="AB51" s="9"/>
     </row>
     <row r="52" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B52">
         <v>-0.35</v>
@@ -4363,14 +4326,14 @@
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
       <c r="I52" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J52" s="11"/>
       <c r="AB52" s="9"/>
     </row>
     <row r="53" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53">
         <v>-0.15</v>
@@ -4379,14 +4342,14 @@
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="I53" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="J53" s="11"/>
       <c r="AB53" s="9"/>
     </row>
     <row r="54" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B54">
         <v>0.1</v>
@@ -4395,7 +4358,7 @@
         <v>17</v>
       </c>
       <c r="I54" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="AB54" s="9"/>
     </row>
@@ -4416,7 +4379,7 @@
         <v>17</v>
       </c>
       <c r="I57" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:126" x14ac:dyDescent="0.2">
@@ -4427,10 +4390,10 @@
         <v>600</v>
       </c>
       <c r="H58" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="I58" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:126" x14ac:dyDescent="0.2">
@@ -4441,10 +4404,10 @@
         <v>20</v>
       </c>
       <c r="H59" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I59" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:126" x14ac:dyDescent="0.2">
@@ -4455,10 +4418,10 @@
         <v>300</v>
       </c>
       <c r="H60" t="s">
+        <v>170</v>
+      </c>
+      <c r="I60" t="s">
         <v>174</v>
-      </c>
-      <c r="I60" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:126" x14ac:dyDescent="0.2">
@@ -4469,10 +4432,10 @@
         <v>970</v>
       </c>
       <c r="H61" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I61" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:126" x14ac:dyDescent="0.2">
@@ -4483,10 +4446,10 @@
         <v>15</v>
       </c>
       <c r="H62" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I62" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:126" x14ac:dyDescent="0.2">
@@ -4497,10 +4460,10 @@
         <v>2</v>
       </c>
       <c r="H63" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I63" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:126" x14ac:dyDescent="0.2">
@@ -4511,13 +4474,13 @@
         <v>380</v>
       </c>
       <c r="H64" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I64" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J64" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.2">
@@ -4528,10 +4491,10 @@
         <v>209</v>
       </c>
       <c r="H65" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I65" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -4551,7 +4514,7 @@
         <v>17</v>
       </c>
       <c r="I68" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="AB68" s="9"/>
     </row>
@@ -4566,7 +4529,7 @@
         <v>17</v>
       </c>
       <c r="I69" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="AB69" s="9"/>
     </row>
@@ -4578,7 +4541,7 @@
         <v>0.3</v>
       </c>
       <c r="I70" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="AB70" s="9"/>
     </row>
@@ -4590,10 +4553,10 @@
         <v>10</v>
       </c>
       <c r="H71" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I71" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="AB71" s="9"/>
     </row>
@@ -4605,7 +4568,7 @@
         <v>0.35</v>
       </c>
       <c r="I72" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="73" spans="1:28" x14ac:dyDescent="0.2">
@@ -4616,7 +4579,7 @@
         <v>20.6</v>
       </c>
       <c r="I73" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="1:28" x14ac:dyDescent="0.2">
@@ -4627,7 +4590,7 @@
         <v>0.2</v>
       </c>
       <c r="I74" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.2">
@@ -4638,7 +4601,7 @@
         <v>0.01</v>
       </c>
       <c r="I75" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.2">
@@ -4649,10 +4612,10 @@
         <v>10</v>
       </c>
       <c r="H76" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I76" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.2">
@@ -4663,10 +4626,10 @@
         <v>0</v>
       </c>
       <c r="H77" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I77" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="79" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -4680,10 +4643,10 @@
         <v>52</v>
       </c>
       <c r="B80" s="9">
-        <v>1.01</v>
+        <v>204.51</v>
       </c>
       <c r="I80" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="AB80" s="9"/>
     </row>
@@ -4692,10 +4655,10 @@
         <v>53</v>
       </c>
       <c r="B81">
-        <v>365.99</v>
+        <v>204.99</v>
       </c>
       <c r="I81" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="AB81" s="9"/>
     </row>
@@ -4704,13 +4667,13 @@
         <v>78</v>
       </c>
       <c r="B82">
-        <v>40.032899999999998</v>
+        <v>53.98</v>
       </c>
       <c r="H82" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I82" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="AB82" s="9"/>
     </row>
@@ -4719,13 +4682,13 @@
         <v>79</v>
       </c>
       <c r="B83">
-        <v>254.45359999999999</v>
+        <v>254.88</v>
       </c>
       <c r="H83" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I83" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="AB83" s="9"/>
     </row>
@@ -4734,65 +4697,79 @@
         <v>80</v>
       </c>
       <c r="B84">
-        <v>-7</v>
+        <v>18</v>
       </c>
       <c r="H84" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I84" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AA86" s="7"/>
     </row>
     <row r="87" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B87" s="9">
         <v>30</v>
       </c>
       <c r="H87" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I87" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="AB87" s="9"/>
     </row>
     <row r="88" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B88" s="9">
         <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I88" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="AB88" s="9"/>
     </row>
     <row r="89" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B89" s="9">
         <v>90</v>
       </c>
       <c r="H89" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I89" t="s">
-        <v>208</v>
+        <v>346</v>
       </c>
       <c r="AB89" s="9"/>
+    </row>
+    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>344</v>
+      </c>
+      <c r="B90" s="9">
+        <v>180</v>
+      </c>
+      <c r="H90" t="s">
+        <v>201</v>
+      </c>
+      <c r="I90" t="s">
+        <v>345</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Added option for fixed viewing azimuth angle
Added an option (dynamic_azimuth) to compute the variable "psi"
(the azimuthal difference between solar and observation angle)
internally in time-series mode based on a fixed observation viewing
angle (called "vazi" in the input data). This modification calls a
new function called calcazimuthangle.m that computes the solar
azimuth angle and psi, the relative difference between that and the
observation angle.
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnorton/Models/SCOPE/SCOPE_v1.73/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5385F807-3183-8A42-B269-F892FB8C6E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD2DCC6-D30C-F84E-B355-06822214AF43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="351">
   <si>
     <t>Cab</t>
   </si>
@@ -1179,6 +1179,9 @@
     <t>CA-OBS-2019</t>
   </si>
   <si>
+    <t>FLEX-S3_std.atm</t>
+  </si>
+  <si>
     <t>calculate the azimuthal difference between solar and observation angle (psi) according to a fixed observation azimuth angle (i.e. psi varies according to the sun-sensor geometry)</t>
   </si>
   <si>
@@ -1192,9 +1195,6 @@
   </si>
   <si>
     <t>azimuthal difference between solar and observation angle  (not used if options.dynamic_azimuth = 1 and options.simulation = 1)</t>
-  </si>
-  <si>
-    <t>FLEX-S3_V80.atm</t>
   </si>
   <si>
     <r>
@@ -1240,6 +1240,12 @@
       </rPr>
       <t>of values for all input that varies between the runs. 1: time series (uses text files with meteo input as time series). 2: Lookup-Table (specify the values to be included. All possible combinations of inputs will be  used)</t>
     </r>
+  </si>
+  <si>
+    <t>sazi</t>
+  </si>
+  <si>
+    <t>solar azimuth angle</t>
   </si>
 </sst>
 </file>
@@ -3120,8 +3126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3346,10 +3352,10 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
+        <v>344</v>
+      </c>
+      <c r="E23" t="s">
         <v>343</v>
-      </c>
-      <c r="E23" t="s">
-        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -3414,7 +3420,7 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3574,10 +3580,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:DV90"/>
+  <dimension ref="A1:DV91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4192,7 +4198,7 @@
         <v>4</v>
       </c>
       <c r="B50" s="9">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="H50" t="s">
         <v>163</v>
@@ -4643,7 +4649,7 @@
         <v>52</v>
       </c>
       <c r="B80" s="9">
-        <v>204.51</v>
+        <v>204.01</v>
       </c>
       <c r="I80" t="s">
         <v>194</v>
@@ -4717,7 +4723,7 @@
         <v>96</v>
       </c>
       <c r="B87" s="9">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H87" t="s">
         <v>201</v>
@@ -4753,13 +4759,13 @@
         <v>201</v>
       </c>
       <c r="I89" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AB89" s="9"/>
     </row>
     <row r="90" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B90" s="9">
         <v>180</v>
@@ -4768,7 +4774,21 @@
         <v>201</v>
       </c>
       <c r="I90" t="s">
-        <v>345</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>349</v>
+      </c>
+      <c r="B91" s="9">
+        <v>0</v>
+      </c>
+      <c r="H91" t="s">
+        <v>201</v>
+      </c>
+      <c r="I91" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added flag for optional prescribed spectra Esun_ Esky_
Added flag option and filename specifications to the input data
files (including xlsx and non-xlsx input files). This flag is
working but does nothing right now.
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnorton/Models/SCOPE/SCOPE_v1.73/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD2DCC6-D30C-F84E-B355-06822214AF43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B6CFB-B7F4-7B4F-BEFE-B870C76B5BBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11780" yWindow="460" windowWidth="21820" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="5" r:id="rId1"/>
@@ -19,19 +19,11 @@
     <sheet name="inputdata" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="357">
   <si>
     <t>Cab</t>
   </si>
@@ -1246,6 +1238,24 @@
   </si>
   <si>
     <t>solar azimuth angle</t>
+  </si>
+  <si>
+    <t>use_prescribed_spectra</t>
+  </si>
+  <si>
+    <t>0: use the MODTRAN atmospheric transfer functions (from "atmos_file") to compute top-of-canopy spectra. 1: use prescribed spectra (one for direct, one for diffuse) as the top-of-canopy spectra</t>
+  </si>
+  <si>
+    <t>Kaniva_hyperspectral_direct.csv</t>
+  </si>
+  <si>
+    <t>Kaniva_hyperspectral_diffuse.csv</t>
+  </si>
+  <si>
+    <t>Esun_spectra_file</t>
+  </si>
+  <si>
+    <t>Esky_spectra_file</t>
   </si>
 </sst>
 </file>
@@ -3124,10 +3134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3358,6 +3368,17 @@
         <v>343</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>351</v>
+      </c>
+      <c r="E24" t="s">
+        <v>352</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3367,10 +3388,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3423,153 +3444,169 @@
         <v>342</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>355</v>
+      </c>
+      <c r="B8" t="s">
+        <v>353</v>
+      </c>
+    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
+        <v>356</v>
+      </c>
+      <c r="B9" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>337</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>65</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="51" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="51" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="B31" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="50" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="50" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="49"/>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3583,7 +3620,7 @@
   <dimension ref="A1:DV91"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4649,7 +4686,7 @@
         <v>52</v>
       </c>
       <c r="B80" s="9">
-        <v>204.01</v>
+        <v>204.48</v>
       </c>
       <c r="I80" t="s">
         <v>194</v>

</xml_diff>

<commit_message>
Reading prescribed spectra directly from file now
By setting the flag use_prescribed_spectra = 1, we now read the
overwrite the Esun_ and Esky_ variables in RTMo.m using input
files. These files are currently hard-coded and have no time-
dependency.
</commit_message>
<xml_diff>
--- a/SCOPE_v1.73/input_data.xlsx
+++ b/SCOPE_v1.73/input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnorton/Models/SCOPE/SCOPE_v1.73/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B6CFB-B7F4-7B4F-BEFE-B870C76B5BBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC00FE72-794F-A84D-843F-EA82E98B8B71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11780" yWindow="460" windowWidth="21820" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="359">
   <si>
     <t>Cab</t>
   </si>
@@ -1256,6 +1256,12 @@
   </si>
   <si>
     <t>Esky_spectra_file</t>
+  </si>
+  <si>
+    <t>testing_prescribed_spectra</t>
+  </si>
+  <si>
+    <t>The_following_are_only_for_the_use_prescribed_spectra_option!</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1708,6 +1714,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3348,7 +3355,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
@@ -3388,10 +3395,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3417,7 +3424,7 @@
         <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>341</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3444,169 +3451,174 @@
         <v>342</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>355</v>
-      </c>
-      <c r="B8" t="s">
-        <v>353</v>
-      </c>
-    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>356</v>
-      </c>
-      <c r="B9" t="s">
-        <v>354</v>
+      <c r="A9" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>56</v>
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>341</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>338</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" t="s">
-        <v>93</v>
+      <c r="A20" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>66</v>
+      <c r="A22" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="51" t="s">
+      <c r="A24" s="51" t="s">
         <v>334</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>59</v>
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>73</v>
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" t="s">
-        <v>340</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="50" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="50" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="49"/>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="49"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="58" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>355</v>
+      </c>
+      <c r="B38" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>356</v>
+      </c>
+      <c r="B39" t="s">
+        <v>354</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>